<commit_message>
update mod1 + mod1.2(uzupelnienie z inne)
</commit_message>
<xml_diff>
--- a/testy_modułów/wynik.xlsx
+++ b/testy_modułów/wynik.xlsx
@@ -10220,7 +10220,11 @@
       <c r="AS73" t="n">
         <v>5310</v>
       </c>
-      <c r="AT73" t="inlineStr"/>
+      <c r="AT73" t="inlineStr">
+        <is>
+          <t>prd.41034900</t>
+        </is>
+      </c>
       <c r="AU73" t="inlineStr"/>
       <c r="AV73" t="inlineStr"/>
       <c r="AW73" t="inlineStr"/>
@@ -10619,7 +10623,11 @@
       <c r="AS76" t="n">
         <v>5310</v>
       </c>
-      <c r="AT76" t="inlineStr"/>
+      <c r="AT76" t="inlineStr">
+        <is>
+          <t>prd.41034903</t>
+        </is>
+      </c>
       <c r="AU76" t="inlineStr"/>
       <c r="AV76" t="inlineStr"/>
       <c r="AW76" t="inlineStr"/>
@@ -13919,7 +13927,11 @@
       <c r="AS101" t="n">
         <v>5310</v>
       </c>
-      <c r="AT101" t="inlineStr"/>
+      <c r="AT101" t="inlineStr">
+        <is>
+          <t>prd.40038124</t>
+        </is>
+      </c>
       <c r="AU101" t="inlineStr"/>
       <c r="AV101" t="inlineStr"/>
       <c r="AW101" t="inlineStr"/>
@@ -14515,7 +14527,11 @@
       <c r="AS105" t="n">
         <v>5310</v>
       </c>
-      <c r="AT105" t="inlineStr"/>
+      <c r="AT105" t="inlineStr">
+        <is>
+          <t>prd.410380334</t>
+        </is>
+      </c>
       <c r="AU105" t="inlineStr"/>
       <c r="AV105" t="inlineStr"/>
       <c r="AW105" t="inlineStr"/>
@@ -28918,7 +28934,11 @@
       <c r="AS219" t="n">
         <v>5310</v>
       </c>
-      <c r="AT219" t="inlineStr"/>
+      <c r="AT219" t="inlineStr">
+        <is>
+          <t>prd.41045201p6i7</t>
+        </is>
+      </c>
       <c r="AU219" t="inlineStr"/>
       <c r="AV219" t="inlineStr"/>
       <c r="AW219" t="inlineStr"/>
@@ -29824,7 +29844,11 @@
       <c r="AS225" t="n">
         <v>5310</v>
       </c>
-      <c r="AT225" t="inlineStr"/>
+      <c r="AT225" t="inlineStr">
+        <is>
+          <t>prd.41045201p6i7</t>
+        </is>
+      </c>
       <c r="AU225" t="inlineStr"/>
       <c r="AV225" t="inlineStr"/>
       <c r="AW225" t="inlineStr"/>
@@ -30312,7 +30336,11 @@
       <c r="AS229" t="n">
         <v>5310</v>
       </c>
-      <c r="AT229" t="inlineStr"/>
+      <c r="AT229" t="inlineStr">
+        <is>
+          <t>prd.41045203</t>
+        </is>
+      </c>
       <c r="AU229" t="inlineStr"/>
       <c r="AV229" t="inlineStr"/>
       <c r="AW229" t="inlineStr"/>
@@ -33331,7 +33359,11 @@
       <c r="AS252" t="n">
         <v>5310</v>
       </c>
-      <c r="AT252" t="inlineStr"/>
+      <c r="AT252" t="inlineStr">
+        <is>
+          <t>prd.40046328</t>
+        </is>
+      </c>
       <c r="AU252" t="inlineStr"/>
       <c r="AV252" t="inlineStr"/>
       <c r="AW252" t="inlineStr"/>
@@ -33597,7 +33629,11 @@
       <c r="AS254" t="n">
         <v>5310</v>
       </c>
-      <c r="AT254" t="inlineStr"/>
+      <c r="AT254" t="inlineStr">
+        <is>
+          <t>prd.SL40046321</t>
+        </is>
+      </c>
       <c r="AU254" t="inlineStr"/>
       <c r="AV254" t="inlineStr"/>
       <c r="AW254" t="inlineStr"/>
@@ -34744,7 +34780,11 @@
       <c r="AS263" t="n">
         <v>5310</v>
       </c>
-      <c r="AT263" t="inlineStr"/>
+      <c r="AT263" t="inlineStr">
+        <is>
+          <t>prd.41046803</t>
+        </is>
+      </c>
       <c r="AU263" t="inlineStr"/>
       <c r="AV263" t="inlineStr"/>
       <c r="AW263" t="inlineStr"/>
@@ -38268,7 +38308,11 @@
       <c r="AS291" t="n">
         <v>5310</v>
       </c>
-      <c r="AT291" t="inlineStr"/>
+      <c r="AT291" t="inlineStr">
+        <is>
+          <t>prd.40051153</t>
+        </is>
+      </c>
       <c r="AU291" t="inlineStr"/>
       <c r="AV291" t="inlineStr"/>
       <c r="AW291" t="inlineStr"/>
@@ -38538,7 +38582,11 @@
       <c r="AS293" t="n">
         <v>5310</v>
       </c>
-      <c r="AT293" t="inlineStr"/>
+      <c r="AT293" t="inlineStr">
+        <is>
+          <t>prd.40051153</t>
+        </is>
+      </c>
       <c r="AU293" t="inlineStr"/>
       <c r="AV293" t="inlineStr"/>
       <c r="AW293" t="inlineStr"/>
@@ -38798,7 +38846,11 @@
       <c r="AS295" t="n">
         <v>5310</v>
       </c>
-      <c r="AT295" t="inlineStr"/>
+      <c r="AT295" t="inlineStr">
+        <is>
+          <t>prd.40051220</t>
+        </is>
+      </c>
       <c r="AU295" t="inlineStr"/>
       <c r="AV295" t="inlineStr"/>
       <c r="AW295" t="inlineStr"/>
@@ -39171,7 +39223,11 @@
       <c r="AS298" t="n">
         <v>5310</v>
       </c>
-      <c r="AT298" t="inlineStr"/>
+      <c r="AT298" t="inlineStr">
+        <is>
+          <t>prd.40051401</t>
+        </is>
+      </c>
       <c r="AU298" t="inlineStr"/>
       <c r="AV298" t="inlineStr"/>
       <c r="AW298" t="inlineStr"/>
@@ -39921,7 +39977,11 @@
       <c r="AS304" t="n">
         <v>5310</v>
       </c>
-      <c r="AT304" t="inlineStr"/>
+      <c r="AT304" t="inlineStr">
+        <is>
+          <t>prd.41051701</t>
+        </is>
+      </c>
       <c r="AU304" t="inlineStr"/>
       <c r="AV304" t="inlineStr"/>
       <c r="AW304" t="inlineStr"/>
@@ -41191,7 +41251,11 @@
       <c r="AS314" t="n">
         <v>5310</v>
       </c>
-      <c r="AT314" t="inlineStr"/>
+      <c r="AT314" t="inlineStr">
+        <is>
+          <t>prd.40051379</t>
+        </is>
+      </c>
       <c r="AU314" t="inlineStr"/>
       <c r="AV314" t="inlineStr"/>
       <c r="AW314" t="inlineStr"/>
@@ -41722,7 +41786,11 @@
       <c r="AS318" t="n">
         <v>5310</v>
       </c>
-      <c r="AT318" t="inlineStr"/>
+      <c r="AT318" t="inlineStr">
+        <is>
+          <t>prd.SL40051380</t>
+        </is>
+      </c>
       <c r="AU318" t="inlineStr"/>
       <c r="AV318" t="inlineStr"/>
       <c r="AW318" t="inlineStr"/>
@@ -43664,7 +43732,11 @@
       <c r="AS333" t="n">
         <v>5310</v>
       </c>
-      <c r="AT333" t="inlineStr"/>
+      <c r="AT333" t="inlineStr">
+        <is>
+          <t>prd.40051220</t>
+        </is>
+      </c>
       <c r="AU333" t="inlineStr"/>
       <c r="AV333" t="inlineStr"/>
       <c r="AW333" t="inlineStr"/>
@@ -45938,7 +46010,11 @@
       <c r="AS351" t="n">
         <v>5310</v>
       </c>
-      <c r="AT351" t="inlineStr"/>
+      <c r="AT351" t="inlineStr">
+        <is>
+          <t>prd.40051220</t>
+        </is>
+      </c>
       <c r="AU351" t="inlineStr"/>
       <c r="AV351" t="inlineStr"/>
       <c r="AW351" t="inlineStr"/>
@@ -46311,7 +46387,11 @@
       <c r="AS354" t="n">
         <v>5310</v>
       </c>
-      <c r="AT354" t="inlineStr"/>
+      <c r="AT354" t="inlineStr">
+        <is>
+          <t>prd.40051401</t>
+        </is>
+      </c>
       <c r="AU354" t="inlineStr"/>
       <c r="AV354" t="inlineStr"/>
       <c r="AW354" t="inlineStr"/>
@@ -48178,7 +48258,11 @@
       <c r="AS369" t="n">
         <v>5310</v>
       </c>
-      <c r="AT369" t="inlineStr"/>
+      <c r="AT369" t="inlineStr">
+        <is>
+          <t>prd.SL41061900</t>
+        </is>
+      </c>
       <c r="AU369" t="inlineStr"/>
       <c r="AV369" t="inlineStr"/>
       <c r="AW369" t="inlineStr"/>
@@ -48434,7 +48518,11 @@
       <c r="AS371" t="n">
         <v>5310</v>
       </c>
-      <c r="AT371" t="inlineStr"/>
+      <c r="AT371" t="inlineStr">
+        <is>
+          <t>prd.41061214</t>
+        </is>
+      </c>
       <c r="AU371" t="inlineStr"/>
       <c r="AV371" t="inlineStr"/>
       <c r="AW371" t="inlineStr"/>
@@ -48690,7 +48778,11 @@
       <c r="AS373" t="n">
         <v>5310</v>
       </c>
-      <c r="AT373" t="inlineStr"/>
+      <c r="AT373" t="inlineStr">
+        <is>
+          <t>prd.41061215</t>
+        </is>
+      </c>
       <c r="AU373" t="inlineStr"/>
       <c r="AV373" t="inlineStr"/>
       <c r="AW373" t="inlineStr"/>
@@ -48946,7 +49038,11 @@
       <c r="AS375" t="n">
         <v>5310</v>
       </c>
-      <c r="AT375" t="inlineStr"/>
+      <c r="AT375" t="inlineStr">
+        <is>
+          <t>prd.40061200</t>
+        </is>
+      </c>
       <c r="AU375" t="inlineStr"/>
       <c r="AV375" t="inlineStr"/>
       <c r="AW375" t="inlineStr"/>
@@ -49807,7 +49903,11 @@
       <c r="AS382" t="n">
         <v>5310</v>
       </c>
-      <c r="AT382" t="inlineStr"/>
+      <c r="AT382" t="inlineStr">
+        <is>
+          <t>prd.SL41061900</t>
+        </is>
+      </c>
       <c r="AU382" t="inlineStr"/>
       <c r="AV382" t="inlineStr"/>
       <c r="AW382" t="inlineStr"/>
@@ -50063,7 +50163,11 @@
       <c r="AS384" t="n">
         <v>5310</v>
       </c>
-      <c r="AT384" t="inlineStr"/>
+      <c r="AT384" t="inlineStr">
+        <is>
+          <t>prd.41061318</t>
+        </is>
+      </c>
       <c r="AU384" t="inlineStr"/>
       <c r="AV384" t="inlineStr"/>
       <c r="AW384" t="inlineStr"/>
@@ -50579,7 +50683,11 @@
       <c r="AS388" t="n">
         <v>5310</v>
       </c>
-      <c r="AT388" t="inlineStr"/>
+      <c r="AT388" t="inlineStr">
+        <is>
+          <t>prd.40061300</t>
+        </is>
+      </c>
       <c r="AU388" t="inlineStr"/>
       <c r="AV388" t="inlineStr"/>
       <c r="AW388" t="inlineStr"/>
@@ -52093,7 +52201,11 @@
       <c r="AS400" t="n">
         <v>5310</v>
       </c>
-      <c r="AT400" t="inlineStr"/>
+      <c r="AT400" t="inlineStr">
+        <is>
+          <t>prd.40062106</t>
+        </is>
+      </c>
       <c r="AU400" t="inlineStr"/>
       <c r="AV400" t="inlineStr"/>
       <c r="AW400" t="inlineStr"/>
@@ -52355,7 +52467,11 @@
       <c r="AS402" t="n">
         <v>5310</v>
       </c>
-      <c r="AT402" t="inlineStr"/>
+      <c r="AT402" t="inlineStr">
+        <is>
+          <t>prd.40062106</t>
+        </is>
+      </c>
       <c r="AU402" t="inlineStr"/>
       <c r="AV402" t="inlineStr"/>
       <c r="AW402" t="inlineStr"/>
@@ -62935,7 +63051,11 @@
       <c r="AS486" t="n">
         <v>5310</v>
       </c>
-      <c r="AT486" t="inlineStr"/>
+      <c r="AT486" t="inlineStr">
+        <is>
+          <t>prd.41085101</t>
+        </is>
+      </c>
       <c r="AU486" t="inlineStr"/>
       <c r="AV486" t="inlineStr"/>
       <c r="AW486" t="inlineStr"/>
@@ -63378,7 +63498,11 @@
       <c r="AS489" t="n">
         <v>5310</v>
       </c>
-      <c r="AT489" t="inlineStr"/>
+      <c r="AT489" t="inlineStr">
+        <is>
+          <t>prd.41085101</t>
+        </is>
+      </c>
       <c r="AU489" t="inlineStr"/>
       <c r="AV489" t="inlineStr"/>
       <c r="AW489" t="inlineStr"/>
@@ -66188,7 +66312,11 @@
       <c r="AS511" t="n">
         <v>5310</v>
       </c>
-      <c r="AT511" t="inlineStr"/>
+      <c r="AT511" t="inlineStr">
+        <is>
+          <t>prd.500173</t>
+        </is>
+      </c>
       <c r="AU511" t="inlineStr"/>
       <c r="AV511" t="inlineStr"/>
       <c r="AW511" t="inlineStr"/>
@@ -66694,7 +66822,11 @@
       <c r="AS515" t="n">
         <v>5310</v>
       </c>
-      <c r="AT515" t="inlineStr"/>
+      <c r="AT515" t="inlineStr">
+        <is>
+          <t>prd.032201</t>
+        </is>
+      </c>
       <c r="AU515" t="inlineStr"/>
       <c r="AV515" t="inlineStr"/>
       <c r="AW515" t="inlineStr"/>
@@ -67559,7 +67691,11 @@
       <c r="AS522" t="n">
         <v>5310</v>
       </c>
-      <c r="AT522" t="inlineStr"/>
+      <c r="AT522" t="inlineStr">
+        <is>
+          <t>prd.032201</t>
+        </is>
+      </c>
       <c r="AU522" t="inlineStr"/>
       <c r="AV522" t="inlineStr"/>
       <c r="AW522" t="inlineStr"/>

</xml_diff>